<commit_message>
bandwidth update and more result related to time
</commit_message>
<xml_diff>
--- a/[3070ti]result.xlsx
+++ b/[3070ti]result.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S12"/>
+  <dimension ref="A1:X28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,15 +510,40 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
+          <t>simulation time(sec)</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>total prepare time(sec)</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>total upload time(sec)</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>total download time(sec)</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>total network delay time(sec)</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
           <t>elapsed time(secs)</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>average upload data(bytes)</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>average download data(bytes)</t>
         </is>
@@ -1181,6 +1206,1192 @@
       </c>
       <c r="S12" s="3" t="n">
         <v>4872</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" t="n">
+        <v>10</v>
+      </c>
+      <c r="E13" t="n">
+        <v>10</v>
+      </c>
+      <c r="F13" t="n">
+        <v>4</v>
+      </c>
+      <c r="G13" t="n">
+        <v>50</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="L13" t="n">
+        <v>2</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="N13" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" s="1" t="n">
+        <v>0.01500781059265137</v>
+      </c>
+      <c r="P13" s="1" t="n">
+        <v>15.00781059265137</v>
+      </c>
+      <c r="Q13" s="2" t="n">
+        <v>11.27304625511169</v>
+      </c>
+      <c r="R13" s="3" t="n">
+        <v>1438.4</v>
+      </c>
+      <c r="S13" s="3" t="n">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" t="n">
+        <v>10</v>
+      </c>
+      <c r="E14" t="n">
+        <v>10</v>
+      </c>
+      <c r="F14" t="n">
+        <v>4</v>
+      </c>
+      <c r="G14" t="n">
+        <v>50</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>10000</v>
+      </c>
+      <c r="L14" t="n">
+        <v>2</v>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="N14" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" s="1" t="n">
+        <v>0.01180830001831055</v>
+      </c>
+      <c r="P14" s="1" t="n">
+        <v>11.80830001831055</v>
+      </c>
+      <c r="Q14" s="2" t="n">
+        <v>10.7666232585907</v>
+      </c>
+      <c r="R14" s="3" t="n">
+        <v>1322.4</v>
+      </c>
+      <c r="S14" s="3" t="n">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" t="n">
+        <v>10</v>
+      </c>
+      <c r="E15" t="n">
+        <v>10</v>
+      </c>
+      <c r="F15" t="n">
+        <v>4</v>
+      </c>
+      <c r="G15" t="n">
+        <v>50</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>10000</v>
+      </c>
+      <c r="L15" t="n">
+        <v>3</v>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="N15" t="n">
+        <v>1</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.01765236854553223</v>
+      </c>
+      <c r="P15" t="n">
+        <v>17.65236854553223</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.01765236854553223</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0.0002439022064208984</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0.011328125</v>
+      </c>
+      <c r="T15" s="1" t="n">
+        <v>0.0056640625</v>
+      </c>
+      <c r="U15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V15" s="2" t="n">
+        <v>10.77872061729431</v>
+      </c>
+      <c r="W15" s="3" t="n">
+        <v>1322.4</v>
+      </c>
+      <c r="X15" s="3" t="n">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" t="n">
+        <v>10</v>
+      </c>
+      <c r="E16" t="n">
+        <v>10</v>
+      </c>
+      <c r="F16" t="n">
+        <v>4</v>
+      </c>
+      <c r="G16" t="n">
+        <v>50</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>10000</v>
+      </c>
+      <c r="L16" t="n">
+        <v>3</v>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="N16" t="n">
+        <v>1</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.01773009300231933</v>
+      </c>
+      <c r="P16" t="n">
+        <v>17.73009300231934</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.01773009300231933</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.0004365444183349609</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0.011328125</v>
+      </c>
+      <c r="T16" s="1" t="n">
+        <v>0.0056640625</v>
+      </c>
+      <c r="U16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V16" s="2" t="n">
+        <v>11.17525696754456</v>
+      </c>
+      <c r="W16" s="3" t="n">
+        <v>1415.2</v>
+      </c>
+      <c r="X16" s="3" t="n">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>2</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" t="n">
+        <v>10</v>
+      </c>
+      <c r="E17" t="n">
+        <v>10</v>
+      </c>
+      <c r="F17" t="n">
+        <v>4</v>
+      </c>
+      <c r="G17" t="n">
+        <v>50</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>10000</v>
+      </c>
+      <c r="L17" t="n">
+        <v>3</v>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="N17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O17" s="1" t="n">
+        <v>0.02830353736877441</v>
+      </c>
+      <c r="P17" s="1" t="n">
+        <v>28.30353736877441</v>
+      </c>
+      <c r="Q17" s="1" t="n">
+        <v>0.02830353736877441</v>
+      </c>
+      <c r="R17" s="1" t="n">
+        <v>0.0008208751678466797</v>
+      </c>
+      <c r="S17" s="1" t="n">
+        <v>0.018125</v>
+      </c>
+      <c r="T17" s="1" t="n">
+        <v>0.009062499999999999</v>
+      </c>
+      <c r="U17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V17" s="2" t="n">
+        <v>11.69054293632507</v>
+      </c>
+      <c r="W17" s="3" t="n">
+        <v>1531.2</v>
+      </c>
+      <c r="X17" s="3" t="n">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>2</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>2</v>
+      </c>
+      <c r="D18" t="n">
+        <v>10</v>
+      </c>
+      <c r="E18" t="n">
+        <v>10</v>
+      </c>
+      <c r="F18" t="n">
+        <v>4</v>
+      </c>
+      <c r="G18" t="n">
+        <v>50</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>10000</v>
+      </c>
+      <c r="L18" t="n">
+        <v>3</v>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="N18" t="n">
+        <v>1</v>
+      </c>
+      <c r="O18" s="1" t="n">
+        <v>0.02176892280578613</v>
+      </c>
+      <c r="P18" s="1" t="n">
+        <v>21.76892280578613</v>
+      </c>
+      <c r="Q18" s="1" t="n">
+        <v>0.02176892280578613</v>
+      </c>
+      <c r="R18" s="1" t="n">
+        <v>0.0005235671997070312</v>
+      </c>
+      <c r="S18" s="1" t="n">
+        <v>0.01359375</v>
+      </c>
+      <c r="T18" s="1" t="n">
+        <v>0.006796875</v>
+      </c>
+      <c r="U18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V18" s="2" t="n">
+        <v>11.48295402526855</v>
+      </c>
+      <c r="W18" s="3" t="n">
+        <v>1484.8</v>
+      </c>
+      <c r="X18" s="3" t="n">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>2</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="n">
+        <v>2</v>
+      </c>
+      <c r="D19" t="n">
+        <v>10</v>
+      </c>
+      <c r="E19" t="n">
+        <v>10</v>
+      </c>
+      <c r="F19" t="n">
+        <v>4</v>
+      </c>
+      <c r="G19" t="n">
+        <v>50</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>1000</v>
+      </c>
+      <c r="L19" t="n">
+        <v>3</v>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="N19" t="n">
+        <v>3</v>
+      </c>
+      <c r="O19" s="1" t="n">
+        <v>0.06074723243713379</v>
+      </c>
+      <c r="P19" s="1" t="n">
+        <v>20.2490774790446</v>
+      </c>
+      <c r="Q19" s="1" t="n">
+        <v>0.06074723243713379</v>
+      </c>
+      <c r="R19" s="1" t="n">
+        <v>0.001528263092041016</v>
+      </c>
+      <c r="S19" s="1" t="n">
+        <v>0.038515625</v>
+      </c>
+      <c r="T19" s="1" t="n">
+        <v>0.0192578125</v>
+      </c>
+      <c r="U19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V19" s="2" t="n">
+        <v>30.88050556182861</v>
+      </c>
+      <c r="W19" s="3" t="n">
+        <v>4152.8</v>
+      </c>
+      <c r="X19" s="3" t="n">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" t="n">
+        <v>10</v>
+      </c>
+      <c r="E20" t="n">
+        <v>10</v>
+      </c>
+      <c r="F20" t="n">
+        <v>4</v>
+      </c>
+      <c r="G20" t="n">
+        <v>50</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>1000</v>
+      </c>
+      <c r="L20" t="n">
+        <v>3</v>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="N20" t="n">
+        <v>4</v>
+      </c>
+      <c r="O20" s="1" t="n">
+        <v>0.07454626083374022</v>
+      </c>
+      <c r="P20" s="1" t="n">
+        <v>18.63656520843506</v>
+      </c>
+      <c r="Q20" s="1" t="n">
+        <v>0.07454626083374022</v>
+      </c>
+      <c r="R20" s="1" t="n">
+        <v>0.001312494277954102</v>
+      </c>
+      <c r="S20" s="1" t="n">
+        <v>0.047578125</v>
+      </c>
+      <c r="T20" s="1" t="n">
+        <v>0.0237890625</v>
+      </c>
+      <c r="U20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V20" s="2" t="n">
+        <v>41.54148554801941</v>
+      </c>
+      <c r="W20" s="3" t="n">
+        <v>5684</v>
+      </c>
+      <c r="X20" s="3" t="n">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="n">
+        <v>2</v>
+      </c>
+      <c r="D21" t="n">
+        <v>10</v>
+      </c>
+      <c r="E21" t="n">
+        <v>10</v>
+      </c>
+      <c r="F21" t="n">
+        <v>4</v>
+      </c>
+      <c r="G21" t="n">
+        <v>50</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" t="n">
+        <v>1000</v>
+      </c>
+      <c r="L21" t="n">
+        <v>10</v>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="N21" t="n">
+        <v>6</v>
+      </c>
+      <c r="O21" s="1" t="n">
+        <v>0.1168572044372559</v>
+      </c>
+      <c r="P21" s="1" t="n">
+        <v>19.47620073954264</v>
+      </c>
+      <c r="Q21" s="1" t="n">
+        <v>0.1168572044372559</v>
+      </c>
+      <c r="R21" s="1" t="n">
+        <v>0.001668691635131836</v>
+      </c>
+      <c r="S21" s="1" t="n">
+        <v>0.074765625</v>
+      </c>
+      <c r="T21" s="1" t="n">
+        <v>0.0373828125</v>
+      </c>
+      <c r="U21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V21" s="2" t="n">
+        <v>60.56818532943726</v>
+      </c>
+      <c r="W21" s="3" t="n">
+        <v>8282.4</v>
+      </c>
+      <c r="X21" s="3" t="n">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="n">
+        <v>2</v>
+      </c>
+      <c r="D22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E22" t="n">
+        <v>10</v>
+      </c>
+      <c r="F22" t="n">
+        <v>4</v>
+      </c>
+      <c r="G22" t="n">
+        <v>50</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>1000</v>
+      </c>
+      <c r="L22" t="n">
+        <v>10</v>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="N22" t="n">
+        <v>8</v>
+      </c>
+      <c r="O22" s="1" t="n">
+        <v>0.1316456699371338</v>
+      </c>
+      <c r="P22" s="1" t="n">
+        <v>16.45570874214172</v>
+      </c>
+      <c r="Q22" s="1" t="n">
+        <v>0.1316456699371338</v>
+      </c>
+      <c r="R22" s="1" t="n">
+        <v>0.001939535140991211</v>
+      </c>
+      <c r="S22" s="1" t="n">
+        <v>0.08382812499999999</v>
+      </c>
+      <c r="T22" s="1" t="n">
+        <v>0.04191406249999999</v>
+      </c>
+      <c r="U22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V22" s="2" t="n">
+        <v>81.28983163833618</v>
+      </c>
+      <c r="W22" s="3" t="n">
+        <v>11252</v>
+      </c>
+      <c r="X22" s="3" t="n">
+        <v>1856</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>2</v>
+      </c>
+      <c r="B23" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" t="n">
+        <v>10</v>
+      </c>
+      <c r="E23" t="n">
+        <v>10</v>
+      </c>
+      <c r="F23" t="n">
+        <v>4</v>
+      </c>
+      <c r="G23" t="n">
+        <v>50</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
+        <v>100</v>
+      </c>
+      <c r="L23" t="n">
+        <v>10</v>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="N23" t="n">
+        <v>6</v>
+      </c>
+      <c r="O23" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="P23" s="1" t="n">
+        <v>15.60525417327881</v>
+      </c>
+      <c r="Q23" s="1" t="n">
+        <v>0.09363152503967284</v>
+      </c>
+      <c r="R23" s="1" t="n">
+        <v>0.001858949661254883</v>
+      </c>
+      <c r="S23" s="1" t="n">
+        <v>0.05890625</v>
+      </c>
+      <c r="T23" s="1" t="n">
+        <v>0.029453125</v>
+      </c>
+      <c r="U23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V23" s="2" t="n">
+        <v>56.23789477348328</v>
+      </c>
+      <c r="W23" s="3" t="n">
+        <v>7284.8</v>
+      </c>
+      <c r="X23" s="3" t="n">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" t="n">
+        <v>2</v>
+      </c>
+      <c r="D24" t="n">
+        <v>10</v>
+      </c>
+      <c r="E24" t="n">
+        <v>10</v>
+      </c>
+      <c r="F24" t="n">
+        <v>4</v>
+      </c>
+      <c r="G24" t="n">
+        <v>50</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" t="n">
+        <v>100</v>
+      </c>
+      <c r="L24" t="n">
+        <v>10</v>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="N24" t="n">
+        <v>6</v>
+      </c>
+      <c r="O24" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="P24" s="1" t="n">
+        <v>17.94268290201823</v>
+      </c>
+      <c r="Q24" s="1" t="n">
+        <v>0.1076560974121094</v>
+      </c>
+      <c r="R24" s="1" t="n">
+        <v>0.001960992813110352</v>
+      </c>
+      <c r="S24" s="1" t="n">
+        <v>0.06796874999999999</v>
+      </c>
+      <c r="T24" s="1" t="n">
+        <v>0.033984375</v>
+      </c>
+      <c r="U24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V24" s="2" t="n">
+        <v>61.45747995376587</v>
+      </c>
+      <c r="W24" s="3" t="n">
+        <v>8491.200000000001</v>
+      </c>
+      <c r="X24" s="3" t="n">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2</v>
+      </c>
+      <c r="B25" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" t="n">
+        <v>10</v>
+      </c>
+      <c r="E25" t="n">
+        <v>10</v>
+      </c>
+      <c r="F25" t="n">
+        <v>4</v>
+      </c>
+      <c r="G25" t="n">
+        <v>50</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" t="n">
+        <v>1000</v>
+      </c>
+      <c r="L25" t="n">
+        <v>10</v>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="N25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O25" s="1" t="n">
+        <v>0.1212155151367187</v>
+      </c>
+      <c r="P25" s="1" t="n">
+        <v>17.31650216238839</v>
+      </c>
+      <c r="Q25" s="1" t="n">
+        <v>0.1212155151367187</v>
+      </c>
+      <c r="R25" s="1" t="n">
+        <v>0.002006292343139648</v>
+      </c>
+      <c r="S25" s="1" t="n">
+        <v>0.07703125</v>
+      </c>
+      <c r="T25" s="1" t="n">
+        <v>0.038515625</v>
+      </c>
+      <c r="U25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V25" s="2" t="n">
+        <v>67.21585321426392</v>
+      </c>
+      <c r="W25" s="3" t="n">
+        <v>8908.799999999999</v>
+      </c>
+      <c r="X25" s="3" t="n">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" t="n">
+        <v>2</v>
+      </c>
+      <c r="D26" t="n">
+        <v>10</v>
+      </c>
+      <c r="E26" t="n">
+        <v>10</v>
+      </c>
+      <c r="F26" t="n">
+        <v>4</v>
+      </c>
+      <c r="G26" t="n">
+        <v>50</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="b">
+        <v>0</v>
+      </c>
+      <c r="K26" t="n">
+        <v>1000</v>
+      </c>
+      <c r="L26" t="n">
+        <v>10</v>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="N26" t="n">
+        <v>8</v>
+      </c>
+      <c r="O26" s="1" t="n">
+        <v>0.1387064743041992</v>
+      </c>
+      <c r="P26" s="1" t="n">
+        <v>17.33830928802491</v>
+      </c>
+      <c r="Q26" s="1" t="n">
+        <v>0.1387064743041992</v>
+      </c>
+      <c r="R26" s="1" t="n">
+        <v>0.001814842224121094</v>
+      </c>
+      <c r="S26" s="1" t="n">
+        <v>0.08835937499999999</v>
+      </c>
+      <c r="T26" s="1" t="n">
+        <v>0.0441796875</v>
+      </c>
+      <c r="U26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V26" s="2" t="n">
+        <v>73.38287830352783</v>
+      </c>
+      <c r="W26" s="3" t="n">
+        <v>9442.4</v>
+      </c>
+      <c r="X26" s="3" t="n">
+        <v>1856</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" t="n">
+        <v>2</v>
+      </c>
+      <c r="D27" t="n">
+        <v>10</v>
+      </c>
+      <c r="E27" t="n">
+        <v>10</v>
+      </c>
+      <c r="F27" t="n">
+        <v>4</v>
+      </c>
+      <c r="G27" t="n">
+        <v>50</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K27" t="n">
+        <v>1000</v>
+      </c>
+      <c r="L27" t="n">
+        <v>10</v>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="N27" t="n">
+        <v>7</v>
+      </c>
+      <c r="O27" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="P27" s="1" t="n">
+        <v>3.200176239013671</v>
+      </c>
+      <c r="Q27" s="1" t="n">
+        <v>0.0224012336730957</v>
+      </c>
+      <c r="R27" s="1" t="n">
+        <v>0.002209186553955078</v>
+      </c>
+      <c r="S27" s="1" t="n">
+        <v>0.010875</v>
+      </c>
+      <c r="T27" s="1" t="n">
+        <v>0.005437500000000001</v>
+      </c>
+      <c r="U27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V27" s="2" t="n">
+        <v>72.8325731754303</v>
+      </c>
+      <c r="W27" s="3" t="n">
+        <v>10208</v>
+      </c>
+      <c r="X27" s="3" t="n">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2</v>
+      </c>
+      <c r="B28" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" t="n">
+        <v>2</v>
+      </c>
+      <c r="D28" t="n">
+        <v>10</v>
+      </c>
+      <c r="E28" t="n">
+        <v>10</v>
+      </c>
+      <c r="F28" t="n">
+        <v>4</v>
+      </c>
+      <c r="G28" t="n">
+        <v>50</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K28" t="n">
+        <v>1000</v>
+      </c>
+      <c r="L28" t="n">
+        <v>10</v>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="N28" t="n">
+        <v>7</v>
+      </c>
+      <c r="O28" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="P28" s="1" t="n">
+        <v>2.603159495762417</v>
+      </c>
+      <c r="Q28" s="1" t="n">
+        <v>0.01822211647033692</v>
+      </c>
+      <c r="R28" s="1" t="n">
+        <v>0.001459598541259766</v>
+      </c>
+      <c r="S28" s="1" t="n">
+        <v>0.008382812500000001</v>
+      </c>
+      <c r="T28" s="1" t="n">
+        <v>0.004191406250000001</v>
+      </c>
+      <c r="U28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V28" s="2" t="n">
+        <v>68.91144251823425</v>
+      </c>
+      <c r="W28" s="3" t="n">
+        <v>9303.200000000001</v>
+      </c>
+      <c r="X28" s="3" t="n">
+        <v>1624</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove file time in prepare section
</commit_message>
<xml_diff>
--- a/[3070ti]result.xlsx
+++ b/[3070ti]result.xlsx
@@ -481,7 +481,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z462"/>
+  <dimension ref="A1:Z474"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -37881,6 +37881,990 @@
         <v>3248</v>
       </c>
     </row>
+    <row r="463">
+      <c r="A463" t="n">
+        <v>2</v>
+      </c>
+      <c r="B463" t="n">
+        <v>1</v>
+      </c>
+      <c r="C463" t="n">
+        <v>2</v>
+      </c>
+      <c r="D463" t="n">
+        <v>10</v>
+      </c>
+      <c r="E463" t="n">
+        <v>10</v>
+      </c>
+      <c r="F463" t="n">
+        <v>3</v>
+      </c>
+      <c r="G463" t="n">
+        <v>50</v>
+      </c>
+      <c r="H463" t="n">
+        <v>0</v>
+      </c>
+      <c r="I463" t="n">
+        <v>0</v>
+      </c>
+      <c r="J463" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K463" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L463" t="b">
+        <v>0</v>
+      </c>
+      <c r="M463" t="n">
+        <v>16</v>
+      </c>
+      <c r="N463" t="n">
+        <v>16</v>
+      </c>
+      <c r="O463" t="inlineStr">
+        <is>
+          <t>&lt;-parameter / result-&gt;</t>
+        </is>
+      </c>
+      <c r="P463" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q463" s="17" t="n">
+        <v>-1</v>
+      </c>
+      <c r="R463" s="17" t="n">
+        <v>2.286108016967773</v>
+      </c>
+      <c r="S463" s="17" t="n">
+        <v>0.009144432067871093</v>
+      </c>
+      <c r="T463" s="17" t="n">
+        <v>0.002155542373657227</v>
+      </c>
+      <c r="U463" s="17" t="n">
+        <v>0.003625</v>
+      </c>
+      <c r="V463" s="17" t="n">
+        <v>0.0018125</v>
+      </c>
+      <c r="W463" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="X463" s="18" t="n">
+        <v>35.2994372844696</v>
+      </c>
+      <c r="Y463" s="19" t="n">
+        <v>4268.8</v>
+      </c>
+      <c r="Z463" s="19" t="n">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="n">
+        <v>2</v>
+      </c>
+      <c r="B464" t="n">
+        <v>1</v>
+      </c>
+      <c r="C464" t="n">
+        <v>2</v>
+      </c>
+      <c r="D464" t="n">
+        <v>10</v>
+      </c>
+      <c r="E464" t="n">
+        <v>10</v>
+      </c>
+      <c r="F464" t="n">
+        <v>3</v>
+      </c>
+      <c r="G464" t="n">
+        <v>50</v>
+      </c>
+      <c r="H464" t="n">
+        <v>0</v>
+      </c>
+      <c r="I464" t="n">
+        <v>0</v>
+      </c>
+      <c r="J464" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K464" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L464" t="b">
+        <v>0</v>
+      </c>
+      <c r="M464" t="n">
+        <v>16</v>
+      </c>
+      <c r="N464" t="n">
+        <v>16</v>
+      </c>
+      <c r="O464" t="inlineStr">
+        <is>
+          <t>&lt;-parameter / result-&gt;</t>
+        </is>
+      </c>
+      <c r="P464" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q464" s="17" t="n">
+        <v>-1</v>
+      </c>
+      <c r="R464" s="17" t="n">
+        <v>2.393219947814941</v>
+      </c>
+      <c r="S464" s="17" t="n">
+        <v>0.009572879791259765</v>
+      </c>
+      <c r="T464" s="17" t="n">
+        <v>0.001131772994995117</v>
+      </c>
+      <c r="U464" s="17" t="n">
+        <v>0.004757812500000001</v>
+      </c>
+      <c r="V464" s="17" t="n">
+        <v>0.00237890625</v>
+      </c>
+      <c r="W464" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="X464" s="18" t="n">
+        <v>37.41122794151306</v>
+      </c>
+      <c r="Y464" s="19" t="n">
+        <v>4756</v>
+      </c>
+      <c r="Z464" s="19" t="n">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="n">
+        <v>2</v>
+      </c>
+      <c r="B465" t="n">
+        <v>1</v>
+      </c>
+      <c r="C465" t="n">
+        <v>2</v>
+      </c>
+      <c r="D465" t="n">
+        <v>10</v>
+      </c>
+      <c r="E465" t="n">
+        <v>10</v>
+      </c>
+      <c r="F465" t="n">
+        <v>3</v>
+      </c>
+      <c r="G465" t="n">
+        <v>50</v>
+      </c>
+      <c r="H465" t="n">
+        <v>0</v>
+      </c>
+      <c r="I465" t="n">
+        <v>0</v>
+      </c>
+      <c r="J465" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K465" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L465" t="b">
+        <v>0</v>
+      </c>
+      <c r="M465" t="n">
+        <v>16</v>
+      </c>
+      <c r="N465" t="n">
+        <v>16</v>
+      </c>
+      <c r="O465" t="inlineStr">
+        <is>
+          <t>&lt;-parameter / result-&gt;</t>
+        </is>
+      </c>
+      <c r="P465" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q465" s="17" t="n">
+        <v>-1</v>
+      </c>
+      <c r="R465" s="17" t="n">
+        <v>2.524171352386475</v>
+      </c>
+      <c r="S465" s="17" t="n">
+        <v>0.0100966854095459</v>
+      </c>
+      <c r="T465" s="17" t="n">
+        <v>0.001620769500732422</v>
+      </c>
+      <c r="U465" s="17" t="n">
+        <v>0.004757812500000001</v>
+      </c>
+      <c r="V465" s="17" t="n">
+        <v>0.00237890625</v>
+      </c>
+      <c r="W465" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="X465" s="18" t="n">
+        <v>37.41674160957336</v>
+      </c>
+      <c r="Y465" s="19" t="n">
+        <v>4756</v>
+      </c>
+      <c r="Z465" s="19" t="n">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="n">
+        <v>2</v>
+      </c>
+      <c r="B466" t="n">
+        <v>1</v>
+      </c>
+      <c r="C466" t="n">
+        <v>2</v>
+      </c>
+      <c r="D466" t="n">
+        <v>10</v>
+      </c>
+      <c r="E466" t="n">
+        <v>10</v>
+      </c>
+      <c r="F466" t="n">
+        <v>3</v>
+      </c>
+      <c r="G466" t="n">
+        <v>50</v>
+      </c>
+      <c r="H466" t="n">
+        <v>0</v>
+      </c>
+      <c r="I466" t="n">
+        <v>0</v>
+      </c>
+      <c r="J466" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K466" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L466" t="b">
+        <v>0</v>
+      </c>
+      <c r="M466" t="n">
+        <v>16</v>
+      </c>
+      <c r="N466" t="n">
+        <v>16</v>
+      </c>
+      <c r="O466" t="inlineStr">
+        <is>
+          <t>&lt;-parameter / result-&gt;</t>
+        </is>
+      </c>
+      <c r="P466" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q466" s="17" t="n">
+        <v>-1</v>
+      </c>
+      <c r="R466" s="17" t="n">
+        <v>2.611611366271973</v>
+      </c>
+      <c r="S466" s="17" t="n">
+        <v>0.01044644546508789</v>
+      </c>
+      <c r="T466" s="17" t="n">
+        <v>0.00184941291809082</v>
+      </c>
+      <c r="U466" s="17" t="n">
+        <v>0.0047578125</v>
+      </c>
+      <c r="V466" s="17" t="n">
+        <v>0.00237890625</v>
+      </c>
+      <c r="W466" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="X466" s="18" t="n">
+        <v>37.41062450408936</v>
+      </c>
+      <c r="Y466" s="19" t="n">
+        <v>4756</v>
+      </c>
+      <c r="Z466" s="19" t="n">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="n">
+        <v>2</v>
+      </c>
+      <c r="B467" t="n">
+        <v>1</v>
+      </c>
+      <c r="C467" t="n">
+        <v>2</v>
+      </c>
+      <c r="D467" t="n">
+        <v>10</v>
+      </c>
+      <c r="E467" t="n">
+        <v>10</v>
+      </c>
+      <c r="F467" t="n">
+        <v>3</v>
+      </c>
+      <c r="G467" t="n">
+        <v>50</v>
+      </c>
+      <c r="H467" t="n">
+        <v>0</v>
+      </c>
+      <c r="I467" t="n">
+        <v>0</v>
+      </c>
+      <c r="J467" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K467" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L467" t="b">
+        <v>0</v>
+      </c>
+      <c r="M467" t="n">
+        <v>16</v>
+      </c>
+      <c r="N467" t="n">
+        <v>16</v>
+      </c>
+      <c r="O467" t="inlineStr">
+        <is>
+          <t>&lt;-parameter / result-&gt;</t>
+        </is>
+      </c>
+      <c r="P467" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q467" s="17" t="n">
+        <v>-1</v>
+      </c>
+      <c r="R467" s="17" t="n">
+        <v>2.542445659637451</v>
+      </c>
+      <c r="S467" s="17" t="n">
+        <v>0.01016978263854981</v>
+      </c>
+      <c r="T467" s="17" t="n">
+        <v>0.001868247985839844</v>
+      </c>
+      <c r="U467" s="17" t="n">
+        <v>0.004531250000000001</v>
+      </c>
+      <c r="V467" s="17" t="n">
+        <v>0.002265625</v>
+      </c>
+      <c r="W467" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="X467" s="18" t="n">
+        <v>38.1127336025238</v>
+      </c>
+      <c r="Y467" s="19" t="n">
+        <v>4918.4</v>
+      </c>
+      <c r="Z467" s="19" t="n">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="n">
+        <v>2</v>
+      </c>
+      <c r="B468" t="n">
+        <v>1</v>
+      </c>
+      <c r="C468" t="n">
+        <v>2</v>
+      </c>
+      <c r="D468" t="n">
+        <v>10</v>
+      </c>
+      <c r="E468" t="n">
+        <v>10</v>
+      </c>
+      <c r="F468" t="n">
+        <v>3</v>
+      </c>
+      <c r="G468" t="n">
+        <v>50</v>
+      </c>
+      <c r="H468" t="n">
+        <v>0</v>
+      </c>
+      <c r="I468" t="n">
+        <v>0</v>
+      </c>
+      <c r="J468" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K468" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L468" t="b">
+        <v>0</v>
+      </c>
+      <c r="M468" t="n">
+        <v>16</v>
+      </c>
+      <c r="N468" t="n">
+        <v>16</v>
+      </c>
+      <c r="O468" t="inlineStr">
+        <is>
+          <t>&lt;-parameter / result-&gt;</t>
+        </is>
+      </c>
+      <c r="P468" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q468" s="17" t="n">
+        <v>-1</v>
+      </c>
+      <c r="R468" s="17" t="n">
+        <v>2.240594387054443</v>
+      </c>
+      <c r="S468" s="17" t="n">
+        <v>0.008962377548217772</v>
+      </c>
+      <c r="T468" s="17" t="n">
+        <v>0.001659870147705078</v>
+      </c>
+      <c r="U468" s="17" t="n">
+        <v>0.0038515625</v>
+      </c>
+      <c r="V468" s="17" t="n">
+        <v>0.00192578125</v>
+      </c>
+      <c r="W468" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="X468" s="18" t="n">
+        <v>37.00537061691284</v>
+      </c>
+      <c r="Y468" s="19" t="n">
+        <v>4663.2</v>
+      </c>
+      <c r="Z468" s="19" t="n">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="n">
+        <v>2</v>
+      </c>
+      <c r="B469" t="n">
+        <v>1</v>
+      </c>
+      <c r="C469" t="n">
+        <v>2</v>
+      </c>
+      <c r="D469" t="n">
+        <v>10</v>
+      </c>
+      <c r="E469" t="n">
+        <v>10</v>
+      </c>
+      <c r="F469" t="n">
+        <v>3</v>
+      </c>
+      <c r="G469" t="n">
+        <v>50</v>
+      </c>
+      <c r="H469" t="n">
+        <v>0</v>
+      </c>
+      <c r="I469" t="n">
+        <v>0</v>
+      </c>
+      <c r="J469" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K469" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L469" t="b">
+        <v>0</v>
+      </c>
+      <c r="M469" t="n">
+        <v>16</v>
+      </c>
+      <c r="N469" t="n">
+        <v>16</v>
+      </c>
+      <c r="O469" t="inlineStr">
+        <is>
+          <t>&lt;-parameter / result-&gt;</t>
+        </is>
+      </c>
+      <c r="P469" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q469" s="17" t="n">
+        <v>-1</v>
+      </c>
+      <c r="R469" s="17" t="n">
+        <v>2.207418918609619</v>
+      </c>
+      <c r="S469" s="17" t="n">
+        <v>0.008829675674438476</v>
+      </c>
+      <c r="T469" s="17" t="n">
+        <v>0.001140594482421875</v>
+      </c>
+      <c r="U469" s="17" t="n">
+        <v>0.004078125</v>
+      </c>
+      <c r="V469" s="17" t="n">
+        <v>0.0020390625</v>
+      </c>
+      <c r="W469" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="X469" s="18" t="n">
+        <v>37.91260147094727</v>
+      </c>
+      <c r="Y469" s="19" t="n">
+        <v>4872</v>
+      </c>
+      <c r="Z469" s="19" t="n">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="n">
+        <v>2</v>
+      </c>
+      <c r="B470" t="n">
+        <v>1</v>
+      </c>
+      <c r="C470" t="n">
+        <v>2</v>
+      </c>
+      <c r="D470" t="n">
+        <v>10</v>
+      </c>
+      <c r="E470" t="n">
+        <v>10</v>
+      </c>
+      <c r="F470" t="n">
+        <v>3</v>
+      </c>
+      <c r="G470" t="n">
+        <v>50</v>
+      </c>
+      <c r="H470" t="n">
+        <v>0</v>
+      </c>
+      <c r="I470" t="n">
+        <v>0</v>
+      </c>
+      <c r="J470" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K470" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L470" t="b">
+        <v>0</v>
+      </c>
+      <c r="M470" t="n">
+        <v>16</v>
+      </c>
+      <c r="N470" t="n">
+        <v>16</v>
+      </c>
+      <c r="O470" t="inlineStr">
+        <is>
+          <t>&lt;-parameter / result-&gt;</t>
+        </is>
+      </c>
+      <c r="P470" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q470" s="17" t="n">
+        <v>-1</v>
+      </c>
+      <c r="R470" s="17" t="n">
+        <v>2.156326770782471</v>
+      </c>
+      <c r="S470" s="17" t="n">
+        <v>0.008625307083129884</v>
+      </c>
+      <c r="T470" s="17" t="n">
+        <v>0.0004904270172119141</v>
+      </c>
+      <c r="U470" s="17" t="n">
+        <v>0.004531250000000001</v>
+      </c>
+      <c r="V470" s="17" t="n">
+        <v>0.002265625</v>
+      </c>
+      <c r="W470" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="X470" s="18" t="n">
+        <v>35.68000936508179</v>
+      </c>
+      <c r="Y470" s="19" t="n">
+        <v>4361.6</v>
+      </c>
+      <c r="Z470" s="19" t="n">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="n">
+        <v>2</v>
+      </c>
+      <c r="B471" t="n">
+        <v>1</v>
+      </c>
+      <c r="C471" t="n">
+        <v>2</v>
+      </c>
+      <c r="D471" t="n">
+        <v>10</v>
+      </c>
+      <c r="E471" t="n">
+        <v>10</v>
+      </c>
+      <c r="F471" t="n">
+        <v>3</v>
+      </c>
+      <c r="G471" t="n">
+        <v>50</v>
+      </c>
+      <c r="H471" t="n">
+        <v>0</v>
+      </c>
+      <c r="I471" t="n">
+        <v>0</v>
+      </c>
+      <c r="J471" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K471" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L471" t="b">
+        <v>0</v>
+      </c>
+      <c r="M471" t="n">
+        <v>16</v>
+      </c>
+      <c r="N471" t="n">
+        <v>16</v>
+      </c>
+      <c r="O471" t="inlineStr">
+        <is>
+          <t>&lt;-parameter / result-&gt;</t>
+        </is>
+      </c>
+      <c r="P471" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q471" s="17" t="n">
+        <v>-1</v>
+      </c>
+      <c r="R471" s="17" t="n">
+        <v>1.548069953918457</v>
+      </c>
+      <c r="S471" s="17" t="n">
+        <v>0.006192279815673829</v>
+      </c>
+      <c r="T471" s="17" t="n">
+        <v>0.0004827976226806641</v>
+      </c>
+      <c r="U471" s="17" t="n">
+        <v>0.0029453125</v>
+      </c>
+      <c r="V471" s="17" t="n">
+        <v>0.00147265625</v>
+      </c>
+      <c r="W471" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="X471" s="18" t="n">
+        <v>34.9842791557312</v>
+      </c>
+      <c r="Y471" s="19" t="n">
+        <v>4199.2</v>
+      </c>
+      <c r="Z471" s="19" t="n">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="n">
+        <v>2</v>
+      </c>
+      <c r="B472" t="n">
+        <v>1</v>
+      </c>
+      <c r="C472" t="n">
+        <v>2</v>
+      </c>
+      <c r="D472" t="n">
+        <v>10</v>
+      </c>
+      <c r="E472" t="n">
+        <v>10</v>
+      </c>
+      <c r="F472" t="n">
+        <v>3</v>
+      </c>
+      <c r="G472" t="n">
+        <v>50</v>
+      </c>
+      <c r="H472" t="n">
+        <v>0</v>
+      </c>
+      <c r="I472" t="n">
+        <v>0</v>
+      </c>
+      <c r="J472" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K472" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L472" t="b">
+        <v>0</v>
+      </c>
+      <c r="M472" t="n">
+        <v>16</v>
+      </c>
+      <c r="N472" t="n">
+        <v>16</v>
+      </c>
+      <c r="O472" t="inlineStr">
+        <is>
+          <t>&lt;-parameter / result-&gt;</t>
+        </is>
+      </c>
+      <c r="P472" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q472" s="17" t="n">
+        <v>-1</v>
+      </c>
+      <c r="R472" s="17" t="n">
+        <v>1.712746620178223</v>
+      </c>
+      <c r="S472" s="17" t="n">
+        <v>0.006850986480712891</v>
+      </c>
+      <c r="T472" s="17" t="n">
+        <v>0.0004765987396240234</v>
+      </c>
+      <c r="U472" s="17" t="n">
+        <v>0.0033984375</v>
+      </c>
+      <c r="V472" s="17" t="n">
+        <v>0.00169921875</v>
+      </c>
+      <c r="W472" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="X472" s="18" t="n">
+        <v>36.80687069892883</v>
+      </c>
+      <c r="Y472" s="19" t="n">
+        <v>4616.8</v>
+      </c>
+      <c r="Z472" s="19" t="n">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="n">
+        <v>2</v>
+      </c>
+      <c r="B473" t="n">
+        <v>1</v>
+      </c>
+      <c r="C473" t="n">
+        <v>2</v>
+      </c>
+      <c r="D473" t="n">
+        <v>10</v>
+      </c>
+      <c r="E473" t="n">
+        <v>10</v>
+      </c>
+      <c r="F473" t="n">
+        <v>3</v>
+      </c>
+      <c r="G473" t="n">
+        <v>50</v>
+      </c>
+      <c r="H473" t="n">
+        <v>0</v>
+      </c>
+      <c r="I473" t="n">
+        <v>0</v>
+      </c>
+      <c r="J473" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K473" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L473" t="b">
+        <v>0</v>
+      </c>
+      <c r="M473" t="n">
+        <v>16</v>
+      </c>
+      <c r="N473" t="n">
+        <v>16</v>
+      </c>
+      <c r="O473" t="inlineStr">
+        <is>
+          <t>&lt;-parameter / result-&gt;</t>
+        </is>
+      </c>
+      <c r="P473" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q473" s="17" t="n">
+        <v>-1</v>
+      </c>
+      <c r="R473" s="17" t="n">
+        <v>2.321778297424316</v>
+      </c>
+      <c r="S473" s="17" t="n">
+        <v>0.009287113189697266</v>
+      </c>
+      <c r="T473" s="17" t="n">
+        <v>0.0004842281341552734</v>
+      </c>
+      <c r="U473" s="17" t="n">
+        <v>0.004984375</v>
+      </c>
+      <c r="V473" s="17" t="n">
+        <v>0.0024921875</v>
+      </c>
+      <c r="W473" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="X473" s="18" t="n">
+        <v>38.35043406486511</v>
+      </c>
+      <c r="Y473" s="19" t="n">
+        <v>4964.8</v>
+      </c>
+      <c r="Z473" s="19" t="n">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="n">
+        <v>2</v>
+      </c>
+      <c r="B474" t="n">
+        <v>1</v>
+      </c>
+      <c r="C474" t="n">
+        <v>2</v>
+      </c>
+      <c r="D474" t="n">
+        <v>10</v>
+      </c>
+      <c r="E474" t="n">
+        <v>10</v>
+      </c>
+      <c r="F474" t="n">
+        <v>3</v>
+      </c>
+      <c r="G474" t="n">
+        <v>50</v>
+      </c>
+      <c r="H474" t="n">
+        <v>0</v>
+      </c>
+      <c r="I474" t="n">
+        <v>0</v>
+      </c>
+      <c r="J474" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K474" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L474" t="b">
+        <v>0</v>
+      </c>
+      <c r="M474" t="n">
+        <v>16</v>
+      </c>
+      <c r="N474" t="n">
+        <v>16</v>
+      </c>
+      <c r="O474" t="inlineStr">
+        <is>
+          <t>&lt;-parameter / result-&gt;</t>
+        </is>
+      </c>
+      <c r="P474" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q474" s="17" t="n">
+        <v>-1</v>
+      </c>
+      <c r="R474" s="17" t="n">
+        <v>1.778490543365479</v>
+      </c>
+      <c r="S474" s="17" t="n">
+        <v>0.007113962173461915</v>
+      </c>
+      <c r="T474" s="17" t="n">
+        <v>0.0006968975067138672</v>
+      </c>
+      <c r="U474" s="17" t="n">
+        <v>0.0033984375</v>
+      </c>
+      <c r="V474" s="17" t="n">
+        <v>0.00169921875</v>
+      </c>
+      <c r="W474" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="X474" s="18" t="n">
+        <v>36.82202172279358</v>
+      </c>
+      <c r="Y474" s="19" t="n">
+        <v>4616.8</v>
+      </c>
+      <c r="Z474" s="19" t="n">
+        <v>928</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add avr pending time
</commit_message>
<xml_diff>
--- a/[3070ti]result.xlsx
+++ b/[3070ti]result.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z9"/>
+  <dimension ref="A1:AA10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -515,45 +515,50 @@
       </c>
       <c r="R1" t="inlineStr">
         <is>
+          <t>average transaction pending time(ms)</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
           <t>average block time(ms)</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>simulation time(sec)</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>total prepare time(sec)</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>total upload time(sec)</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>total download time(sec)</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>total network delay time(sec)</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>elapsed time(secs)</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>average upload data(bytes)</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>average download data(bytes)</t>
         </is>
@@ -1213,6 +1218,91 @@
       </c>
       <c r="Z9" s="3" t="n">
         <v>2552</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>10</v>
+      </c>
+      <c r="E10" t="n">
+        <v>10</v>
+      </c>
+      <c r="F10" t="n">
+        <v>3</v>
+      </c>
+      <c r="G10" t="n">
+        <v>50</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>100</v>
+      </c>
+      <c r="K10" t="n">
+        <v>200</v>
+      </c>
+      <c r="L10" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>16384</v>
+      </c>
+      <c r="N10" t="n">
+        <v>40</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>&lt;-parameter / result-&gt;</t>
+        </is>
+      </c>
+      <c r="P10" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.2623854160308838</v>
+      </c>
+      <c r="R10" s="1" t="n">
+        <v>111.4573558330536</v>
+      </c>
+      <c r="S10" s="1" t="n">
+        <v>26.23854160308838</v>
+      </c>
+      <c r="T10" s="1" t="n">
+        <v>0.2623854160308838</v>
+      </c>
+      <c r="U10" s="1" t="n">
+        <v>0.0001642704010009766</v>
+      </c>
+      <c r="V10" s="1" t="n">
+        <v>0.090625</v>
+      </c>
+      <c r="W10" s="1" t="n">
+        <v>0.0453125</v>
+      </c>
+      <c r="X10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="2" t="n">
+        <v>94.52276921272278</v>
+      </c>
+      <c r="Z10" s="3" t="n">
+        <v>12528</v>
+      </c>
+      <c r="AA10" s="3" t="n">
+        <v>2320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix avr pending time
</commit_message>
<xml_diff>
--- a/[3070ti]result.xlsx
+++ b/[3070ti]result.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA10"/>
+  <dimension ref="A1:AA12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1305,6 +1305,176 @@
         <v>2320</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" t="n">
+        <v>10</v>
+      </c>
+      <c r="E11" t="n">
+        <v>10</v>
+      </c>
+      <c r="F11" t="n">
+        <v>3</v>
+      </c>
+      <c r="G11" t="n">
+        <v>50</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>100</v>
+      </c>
+      <c r="K11" t="n">
+        <v>200</v>
+      </c>
+      <c r="L11" t="b">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>16384</v>
+      </c>
+      <c r="N11" t="n">
+        <v>40</v>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>&lt;-parameter / result-&gt;</t>
+        </is>
+      </c>
+      <c r="P11" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q11" s="1" t="n">
+        <v>0.2571566200256348</v>
+      </c>
+      <c r="R11" s="1" t="n">
+        <v>111.4790219664574</v>
+      </c>
+      <c r="S11" s="1" t="n">
+        <v>32.14457750320435</v>
+      </c>
+      <c r="T11" s="1" t="n">
+        <v>0.2571566200256348</v>
+      </c>
+      <c r="U11" s="1" t="n">
+        <v>0.00058746337890625</v>
+      </c>
+      <c r="V11" s="1" t="n">
+        <v>0.08609374999999998</v>
+      </c>
+      <c r="W11" s="1" t="n">
+        <v>0.04304687499999999</v>
+      </c>
+      <c r="X11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="2" t="n">
+        <v>70.0704345703125</v>
+      </c>
+      <c r="Z11" s="3" t="n">
+        <v>8676.799999999999</v>
+      </c>
+      <c r="AA11" s="3" t="n">
+        <v>1856</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" t="n">
+        <v>10</v>
+      </c>
+      <c r="E12" t="n">
+        <v>10</v>
+      </c>
+      <c r="F12" t="n">
+        <v>3</v>
+      </c>
+      <c r="G12" t="n">
+        <v>100</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>100</v>
+      </c>
+      <c r="K12" t="n">
+        <v>200</v>
+      </c>
+      <c r="L12" t="b">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>32768</v>
+      </c>
+      <c r="N12" t="n">
+        <v>95</v>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>&lt;-parameter / result-&gt;</t>
+        </is>
+      </c>
+      <c r="P12" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q12" s="1" t="n">
+        <v>0.5498097991943359</v>
+      </c>
+      <c r="R12" s="1" t="n">
+        <v>245.275257277907</v>
+      </c>
+      <c r="S12" s="1" t="n">
+        <v>36.65398661295573</v>
+      </c>
+      <c r="T12" s="1" t="n">
+        <v>0.5498097991943359</v>
+      </c>
+      <c r="U12" s="1" t="n">
+        <v>0.0004422664642333984</v>
+      </c>
+      <c r="V12" s="1" t="n">
+        <v>0.1540625</v>
+      </c>
+      <c r="W12" s="1" t="n">
+        <v>0.07703125</v>
+      </c>
+      <c r="X12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="2" t="n">
+        <v>140.8762097358704</v>
+      </c>
+      <c r="Z12" s="3" t="n">
+        <v>17585.6</v>
+      </c>
+      <c r="AA12" s="3" t="n">
+        <v>3480</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
optimize init time by just print a new line when read json
</commit_message>
<xml_diff>
--- a/[3070ti]result.xlsx
+++ b/[3070ti]result.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC294"/>
+  <dimension ref="A1:AC302"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -27237,6 +27237,734 @@
         <v>0</v>
       </c>
     </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>2</v>
+      </c>
+      <c r="B295" t="n">
+        <v>1</v>
+      </c>
+      <c r="C295" t="n">
+        <v>2</v>
+      </c>
+      <c r="D295" t="n">
+        <v>10</v>
+      </c>
+      <c r="E295" t="n">
+        <v>10</v>
+      </c>
+      <c r="F295" t="n">
+        <v>3</v>
+      </c>
+      <c r="G295" t="n">
+        <v>50</v>
+      </c>
+      <c r="H295" t="n">
+        <v>0</v>
+      </c>
+      <c r="I295" t="n">
+        <v>0</v>
+      </c>
+      <c r="J295" t="n">
+        <v>100</v>
+      </c>
+      <c r="K295" t="n">
+        <v>200</v>
+      </c>
+      <c r="L295" t="b">
+        <v>0</v>
+      </c>
+      <c r="M295" t="n">
+        <v>-2</v>
+      </c>
+      <c r="N295" t="n">
+        <v>100</v>
+      </c>
+      <c r="O295" t="n">
+        <v>256</v>
+      </c>
+      <c r="P295" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q295" t="inlineStr">
+        <is>
+          <t>&lt;-parameter / result-&gt;</t>
+        </is>
+      </c>
+      <c r="R295" t="n">
+        <v>8</v>
+      </c>
+      <c r="S295" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="T295" s="1" t="n">
+        <v>40.37446797688803</v>
+      </c>
+      <c r="U295" s="1" t="n">
+        <v>13.95394086837769</v>
+      </c>
+      <c r="V295" s="1" t="n">
+        <v>0.1116315269470215</v>
+      </c>
+      <c r="W295" s="1" t="n">
+        <v>8.034706115722656e-05</v>
+      </c>
+      <c r="X295" s="1" t="n">
+        <v>0.0725</v>
+      </c>
+      <c r="Y295" s="1" t="n">
+        <v>0.03625</v>
+      </c>
+      <c r="Z295" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA295" s="2" t="n">
+        <v>1.221457004547119</v>
+      </c>
+      <c r="AB295" s="3" t="n">
+        <v>742.4</v>
+      </c>
+      <c r="AC295" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>2</v>
+      </c>
+      <c r="B296" t="n">
+        <v>1</v>
+      </c>
+      <c r="C296" t="n">
+        <v>2</v>
+      </c>
+      <c r="D296" t="n">
+        <v>10</v>
+      </c>
+      <c r="E296" t="n">
+        <v>10</v>
+      </c>
+      <c r="F296" t="n">
+        <v>3</v>
+      </c>
+      <c r="G296" t="n">
+        <v>50</v>
+      </c>
+      <c r="H296" t="n">
+        <v>0</v>
+      </c>
+      <c r="I296" t="n">
+        <v>0</v>
+      </c>
+      <c r="J296" t="n">
+        <v>100</v>
+      </c>
+      <c r="K296" t="n">
+        <v>200</v>
+      </c>
+      <c r="L296" t="b">
+        <v>0</v>
+      </c>
+      <c r="M296" t="n">
+        <v>-2</v>
+      </c>
+      <c r="N296" t="n">
+        <v>100</v>
+      </c>
+      <c r="O296" t="n">
+        <v>600</v>
+      </c>
+      <c r="P296" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q296" t="inlineStr">
+        <is>
+          <t>&lt;-parameter / result-&gt;</t>
+        </is>
+      </c>
+      <c r="R296" t="n">
+        <v>5</v>
+      </c>
+      <c r="S296" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="T296" s="1" t="n">
+        <v>29.42369191542915</v>
+      </c>
+      <c r="U296" s="1" t="n">
+        <v>17.55800247192383</v>
+      </c>
+      <c r="V296" s="1" t="n">
+        <v>0.08779001235961914</v>
+      </c>
+      <c r="W296" s="1" t="n">
+        <v>7.033348083496094e-05</v>
+      </c>
+      <c r="X296" s="1" t="n">
+        <v>0.056640625</v>
+      </c>
+      <c r="Y296" s="1" t="n">
+        <v>0.0283203125</v>
+      </c>
+      <c r="Z296" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA296" s="2" t="n">
+        <v>1.223086357116699</v>
+      </c>
+      <c r="AB296" s="3" t="n">
+        <v>580</v>
+      </c>
+      <c r="AC296" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>2</v>
+      </c>
+      <c r="B297" t="n">
+        <v>1</v>
+      </c>
+      <c r="C297" t="n">
+        <v>2</v>
+      </c>
+      <c r="D297" t="n">
+        <v>10</v>
+      </c>
+      <c r="E297" t="n">
+        <v>10</v>
+      </c>
+      <c r="F297" t="n">
+        <v>3</v>
+      </c>
+      <c r="G297" t="n">
+        <v>50</v>
+      </c>
+      <c r="H297" t="n">
+        <v>0</v>
+      </c>
+      <c r="I297" t="n">
+        <v>0</v>
+      </c>
+      <c r="J297" t="n">
+        <v>100</v>
+      </c>
+      <c r="K297" t="n">
+        <v>200</v>
+      </c>
+      <c r="L297" t="b">
+        <v>0</v>
+      </c>
+      <c r="M297" t="n">
+        <v>-2</v>
+      </c>
+      <c r="N297" t="n">
+        <v>100</v>
+      </c>
+      <c r="O297" t="n">
+        <v>256</v>
+      </c>
+      <c r="P297" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q297" t="inlineStr">
+        <is>
+          <t>&lt;-parameter / result-&gt;</t>
+        </is>
+      </c>
+      <c r="R297" t="n">
+        <v>9</v>
+      </c>
+      <c r="S297" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="T297" s="1" t="n">
+        <v>51.1702262654024</v>
+      </c>
+      <c r="U297" s="1" t="n">
+        <v>17.50065485636394</v>
+      </c>
+      <c r="V297" s="1" t="n">
+        <v>0.1575058937072754</v>
+      </c>
+      <c r="W297" s="1" t="n">
+        <v>0.0001037120819091797</v>
+      </c>
+      <c r="X297" s="1" t="n">
+        <v>0.101953125</v>
+      </c>
+      <c r="Y297" s="1" t="n">
+        <v>0.05097656249999999</v>
+      </c>
+      <c r="Z297" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA297" s="2" t="n">
+        <v>1.225745677947998</v>
+      </c>
+      <c r="AB297" s="3" t="n">
+        <v>1044</v>
+      </c>
+      <c r="AC297" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>2</v>
+      </c>
+      <c r="B298" t="n">
+        <v>1</v>
+      </c>
+      <c r="C298" t="n">
+        <v>2</v>
+      </c>
+      <c r="D298" t="n">
+        <v>10</v>
+      </c>
+      <c r="E298" t="n">
+        <v>10</v>
+      </c>
+      <c r="F298" t="n">
+        <v>3</v>
+      </c>
+      <c r="G298" t="n">
+        <v>50</v>
+      </c>
+      <c r="H298" t="n">
+        <v>0</v>
+      </c>
+      <c r="I298" t="n">
+        <v>0</v>
+      </c>
+      <c r="J298" t="n">
+        <v>100</v>
+      </c>
+      <c r="K298" t="n">
+        <v>200</v>
+      </c>
+      <c r="L298" t="b">
+        <v>0</v>
+      </c>
+      <c r="M298" t="n">
+        <v>-2</v>
+      </c>
+      <c r="N298" t="n">
+        <v>100</v>
+      </c>
+      <c r="O298" t="n">
+        <v>256</v>
+      </c>
+      <c r="P298" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q298" t="inlineStr">
+        <is>
+          <t>&lt;-parameter / result-&gt;</t>
+        </is>
+      </c>
+      <c r="R298" t="n">
+        <v>9</v>
+      </c>
+      <c r="S298" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="T298" s="1" t="n">
+        <v>50.4506430906408</v>
+      </c>
+      <c r="U298" s="1" t="n">
+        <v>17.42459932963054</v>
+      </c>
+      <c r="V298" s="1" t="n">
+        <v>0.1568213939666748</v>
+      </c>
+      <c r="W298" s="1" t="n">
+        <v>9.751319885253906e-05</v>
+      </c>
+      <c r="X298" s="1" t="n">
+        <v>0.101953125</v>
+      </c>
+      <c r="Y298" s="1" t="n">
+        <v>0.05097656249999999</v>
+      </c>
+      <c r="Z298" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA298" s="2" t="n">
+        <v>1.224261045455933</v>
+      </c>
+      <c r="AB298" s="3" t="n">
+        <v>1044</v>
+      </c>
+      <c r="AC298" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>2</v>
+      </c>
+      <c r="B299" t="n">
+        <v>1</v>
+      </c>
+      <c r="C299" t="n">
+        <v>2</v>
+      </c>
+      <c r="D299" t="n">
+        <v>10</v>
+      </c>
+      <c r="E299" t="n">
+        <v>10</v>
+      </c>
+      <c r="F299" t="n">
+        <v>3</v>
+      </c>
+      <c r="G299" t="n">
+        <v>50</v>
+      </c>
+      <c r="H299" t="n">
+        <v>0</v>
+      </c>
+      <c r="I299" t="n">
+        <v>0</v>
+      </c>
+      <c r="J299" t="n">
+        <v>100</v>
+      </c>
+      <c r="K299" t="n">
+        <v>200</v>
+      </c>
+      <c r="L299" t="b">
+        <v>0</v>
+      </c>
+      <c r="M299" t="n">
+        <v>-2</v>
+      </c>
+      <c r="N299" t="n">
+        <v>100</v>
+      </c>
+      <c r="O299" t="n">
+        <v>256</v>
+      </c>
+      <c r="P299" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q299" t="inlineStr">
+        <is>
+          <t>&lt;-parameter / result-&gt;</t>
+        </is>
+      </c>
+      <c r="R299" t="n">
+        <v>7</v>
+      </c>
+      <c r="S299" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="T299" s="1" t="n">
+        <v>32.62987295786539</v>
+      </c>
+      <c r="U299" s="1" t="n">
+        <v>10.87885856628418</v>
+      </c>
+      <c r="V299" s="1" t="n">
+        <v>0.07615200996398924</v>
+      </c>
+      <c r="W299" s="1" t="n">
+        <v>7.367134094238281e-05</v>
+      </c>
+      <c r="X299" s="1" t="n">
+        <v>0.047578125</v>
+      </c>
+      <c r="Y299" s="1" t="n">
+        <v>0.0237890625</v>
+      </c>
+      <c r="Z299" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA299" s="2" t="n">
+        <v>1.223163843154907</v>
+      </c>
+      <c r="AB299" s="3" t="n">
+        <v>487.2</v>
+      </c>
+      <c r="AC299" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>2</v>
+      </c>
+      <c r="B300" t="n">
+        <v>1</v>
+      </c>
+      <c r="C300" t="n">
+        <v>2</v>
+      </c>
+      <c r="D300" t="n">
+        <v>10</v>
+      </c>
+      <c r="E300" t="n">
+        <v>10</v>
+      </c>
+      <c r="F300" t="n">
+        <v>3</v>
+      </c>
+      <c r="G300" t="n">
+        <v>50</v>
+      </c>
+      <c r="H300" t="n">
+        <v>0</v>
+      </c>
+      <c r="I300" t="n">
+        <v>0</v>
+      </c>
+      <c r="J300" t="n">
+        <v>100</v>
+      </c>
+      <c r="K300" t="n">
+        <v>200</v>
+      </c>
+      <c r="L300" t="b">
+        <v>0</v>
+      </c>
+      <c r="M300" t="n">
+        <v>-2</v>
+      </c>
+      <c r="N300" t="n">
+        <v>100</v>
+      </c>
+      <c r="O300" t="n">
+        <v>256</v>
+      </c>
+      <c r="P300" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q300" t="inlineStr">
+        <is>
+          <t>&lt;-parameter / result-&gt;</t>
+        </is>
+      </c>
+      <c r="R300" t="n">
+        <v>9</v>
+      </c>
+      <c r="S300" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="T300" s="1" t="n">
+        <v>51.25487888560576</v>
+      </c>
+      <c r="U300" s="1" t="n">
+        <v>17.52092043558757</v>
+      </c>
+      <c r="V300" s="1" t="n">
+        <v>0.1576882839202881</v>
+      </c>
+      <c r="W300" s="1" t="n">
+        <v>0.0001018047332763672</v>
+      </c>
+      <c r="X300" s="1" t="n">
+        <v>0.101953125</v>
+      </c>
+      <c r="Y300" s="1" t="n">
+        <v>0.05097656249999999</v>
+      </c>
+      <c r="Z300" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA300" s="2" t="n">
+        <v>1.225343465805054</v>
+      </c>
+      <c r="AB300" s="3" t="n">
+        <v>1044</v>
+      </c>
+      <c r="AC300" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>2</v>
+      </c>
+      <c r="B301" t="n">
+        <v>1</v>
+      </c>
+      <c r="C301" t="n">
+        <v>2</v>
+      </c>
+      <c r="D301" t="n">
+        <v>10</v>
+      </c>
+      <c r="E301" t="n">
+        <v>10</v>
+      </c>
+      <c r="F301" t="n">
+        <v>3</v>
+      </c>
+      <c r="G301" t="n">
+        <v>50</v>
+      </c>
+      <c r="H301" t="n">
+        <v>0</v>
+      </c>
+      <c r="I301" t="n">
+        <v>0</v>
+      </c>
+      <c r="J301" t="n">
+        <v>100</v>
+      </c>
+      <c r="K301" t="n">
+        <v>200</v>
+      </c>
+      <c r="L301" t="b">
+        <v>0</v>
+      </c>
+      <c r="M301" t="n">
+        <v>-2</v>
+      </c>
+      <c r="N301" t="n">
+        <v>100</v>
+      </c>
+      <c r="O301" t="n">
+        <v>256</v>
+      </c>
+      <c r="P301" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q301" t="inlineStr">
+        <is>
+          <t>&lt;-parameter / result-&gt;</t>
+        </is>
+      </c>
+      <c r="R301" t="n">
+        <v>9</v>
+      </c>
+      <c r="S301" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="T301" s="1" t="n">
+        <v>51.34789298562442</v>
+      </c>
+      <c r="U301" s="1" t="n">
+        <v>17.51774152119955</v>
+      </c>
+      <c r="V301" s="1" t="n">
+        <v>0.1576596736907959</v>
+      </c>
+      <c r="W301" s="1" t="n">
+        <v>9.059906005859375e-05</v>
+      </c>
+      <c r="X301" s="1" t="n">
+        <v>0.101953125</v>
+      </c>
+      <c r="Y301" s="1" t="n">
+        <v>0.05097656249999999</v>
+      </c>
+      <c r="Z301" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA301" s="2" t="n">
+        <v>1.224569797515869</v>
+      </c>
+      <c r="AB301" s="3" t="n">
+        <v>1044</v>
+      </c>
+      <c r="AC301" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>2</v>
+      </c>
+      <c r="B302" t="n">
+        <v>1</v>
+      </c>
+      <c r="C302" t="n">
+        <v>2</v>
+      </c>
+      <c r="D302" t="n">
+        <v>10</v>
+      </c>
+      <c r="E302" t="n">
+        <v>10</v>
+      </c>
+      <c r="F302" t="n">
+        <v>3</v>
+      </c>
+      <c r="G302" t="n">
+        <v>50</v>
+      </c>
+      <c r="H302" t="n">
+        <v>0</v>
+      </c>
+      <c r="I302" t="n">
+        <v>0</v>
+      </c>
+      <c r="J302" t="n">
+        <v>100</v>
+      </c>
+      <c r="K302" t="n">
+        <v>200</v>
+      </c>
+      <c r="L302" t="b">
+        <v>0</v>
+      </c>
+      <c r="M302" t="n">
+        <v>-2</v>
+      </c>
+      <c r="N302" t="n">
+        <v>100</v>
+      </c>
+      <c r="O302" t="n">
+        <v>256</v>
+      </c>
+      <c r="P302" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q302" t="inlineStr">
+        <is>
+          <t>&lt;-parameter / result-&gt;</t>
+        </is>
+      </c>
+      <c r="R302" t="n">
+        <v>7</v>
+      </c>
+      <c r="S302" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="T302" s="1" t="n">
+        <v>31.04332923889159</v>
+      </c>
+      <c r="U302" s="1" t="n">
+        <v>10.54476601736886</v>
+      </c>
+      <c r="V302" s="1" t="n">
+        <v>0.07381336212158202</v>
+      </c>
+      <c r="W302" s="1" t="n">
+        <v>7.486343383789062e-05</v>
+      </c>
+      <c r="X302" s="1" t="n">
+        <v>0.047578125</v>
+      </c>
+      <c r="Y302" s="1" t="n">
+        <v>0.0237890625</v>
+      </c>
+      <c r="Z302" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA302" s="2" t="n">
+        <v>1.221666812896729</v>
+      </c>
+      <c r="AB302" s="3" t="n">
+        <v>487.2</v>
+      </c>
+      <c r="AC302" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>